<commit_message>
added untested unpipelined processor, fixed controls and other small bugs
</commit_message>
<xml_diff>
--- a/cpu_upl/controls.xlsx
+++ b/cpu_upl/controls.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Instruction</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>101</t>
+  </si>
+  <si>
+    <t>ctrl_alu_dmem</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,9 +542,10 @@
     <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -584,8 +588,11 @@
       <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -625,8 +632,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -666,8 +676,11 @@
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -707,8 +720,11 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -748,8 +764,11 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -789,8 +808,11 @@
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -830,8 +852,11 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -871,8 +896,11 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -912,8 +940,11 @@
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -953,8 +984,11 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -994,8 +1028,11 @@
       <c r="M11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1035,8 +1072,11 @@
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1076,8 +1116,11 @@
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1117,8 +1160,11 @@
       <c r="M14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1158,8 +1204,11 @@
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1199,8 +1248,11 @@
       <c r="M16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1239,6 +1291,9 @@
       </c>
       <c r="M17">
         <v>1</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debugging outputs on the processor and fixes to the control block. regfile is not working
</commit_message>
<xml_diff>
--- a/cpu_upl/controls.xlsx
+++ b/cpu_upl/controls.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Instruction</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>ctrl_alu_dmem</t>
+  </si>
+  <si>
+    <t>ctrl_reg_input_mux</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +548,7 @@
     <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,8 +594,11 @@
       <c r="O1" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -635,8 +641,11 @@
       <c r="O2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -679,8 +688,11 @@
       <c r="O3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -723,8 +735,11 @@
       <c r="O4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -767,8 +782,11 @@
       <c r="O5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -811,8 +829,11 @@
       <c r="O6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -855,8 +876,11 @@
       <c r="O7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -899,8 +923,11 @@
       <c r="O8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -943,8 +970,11 @@
       <c r="O9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -987,8 +1017,11 @@
       <c r="O10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1031,8 +1064,11 @@
       <c r="O11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1075,8 +1111,11 @@
       <c r="O12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1119,8 +1158,11 @@
       <c r="O13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1163,8 +1205,11 @@
       <c r="O14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1207,8 +1252,11 @@
       <c r="O15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1251,8 +1299,11 @@
       <c r="O16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1293,6 +1344,9 @@
         <v>1</v>
       </c>
       <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added mux for $rt and $rd into regfile's second read port, which is necessary for lw, sw, beq, and bgt. added signals for alu_isGreater and alu_isEqual.
</commit_message>
<xml_diff>
--- a/cpu_upl/controls.xlsx
+++ b/cpu_upl/controls.xlsx
@@ -27,9 +27,6 @@
     <t>ctrl_reg_reset</t>
   </si>
   <si>
-    <t>ctrl_dest_mux</t>
-  </si>
-  <si>
     <t>ctrl_sign_ex_mux</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>ctrl_reg_input_mux</t>
+  </si>
+  <si>
+    <t>ctrl_rt_mux</t>
   </si>
 </sst>
 </file>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,8 @@
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
@@ -553,7 +554,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -562,48 +563,48 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="O1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -612,13 +613,13 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -647,10 +648,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -659,13 +660,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -694,10 +695,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -706,13 +707,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -741,10 +742,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -753,13 +754,13 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -788,10 +789,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -800,13 +801,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -835,10 +836,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -847,13 +848,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -882,10 +883,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -900,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -929,10 +930,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -941,13 +942,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -976,10 +977,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -988,13 +989,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1023,10 +1024,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1035,13 +1036,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1070,10 +1071,10 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1082,13 +1083,13 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1117,10 +1118,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1135,7 +1136,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1164,10 +1165,10 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1182,7 +1183,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1211,10 +1212,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1229,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1258,10 +1259,10 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1276,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1305,25 +1306,25 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="H17">
         <v>0</v>

</xml_diff>

<commit_message>
fixed compilation errors. processor_ppl is only partially complete but it compiles.
</commit_message>
<xml_diff>
--- a/cpu_upl/controls.xlsx
+++ b/cpu_upl/controls.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>44</v>
@@ -1086,7 +1086,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>44</v>

</xml_diff>